<commit_message>
Layout v1 png, further development on site
</commit_message>
<xml_diff>
--- a/DOM.xlsx
+++ b/DOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/362c63ac4c07b5d2/School/SDU/Læringsteknologi/Semesterprojekt3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{C244615C-42E3-4C4C-8924-44CF9A7D71E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34CBD328-EBB7-493A-BC3A-171BD3104455}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{C244615C-42E3-4C4C-8924-44CF9A7D71E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94DA6178-46A5-45F0-A848-904A2D8E36AC}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="38700" windowHeight="15345" xr2:uid="{AA7C7382-57C4-47AB-84A6-BFBF8ED1522F}"/>
   </bookViews>
@@ -93,10 +93,10 @@
     <t>Page</t>
   </si>
   <si>
-    <t>Column2</t>
-  </si>
-  <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Content</t>
   </si>
 </sst>
 </file>
@@ -166,7 +166,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{92269BA4-4C44-4484-8150-DA5983A6C087}" name="Done"/>
     <tableColumn id="2" xr3:uid="{1253ED7C-26AB-4DF0-9FBA-36B8CD4C5854}" name="Page"/>
-    <tableColumn id="3" xr3:uid="{4E39359E-6FF3-4B38-9EA9-618FB21E8F7C}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{4E39359E-6FF3-4B38-9EA9-618FB21E8F7C}" name="Content"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -472,7 +472,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,13 +484,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>